<commit_message>
fix: tampilan, tombol & template
</commit_message>
<xml_diff>
--- a/POS/public/template_level.xlsx
+++ b/POS/public/template_level.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_2025\Minggu8\PWL_POS\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_2025\POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D47A3D0-6462-4790-8B1D-6C9777659F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DD17DB-5F9E-491D-8C6B-BBBE52B8D00A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{1596EF16-456D-4292-87C3-1EEC05AD2721}"/>
+    <workbookView xWindow="3630" yWindow="3630" windowWidth="21600" windowHeight="11295" xr2:uid="{1596EF16-456D-4292-87C3-1EEC05AD2721}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,10 @@
     <t>level_nama</t>
   </si>
   <si>
-    <t>CTM</t>
+    <t>MBR</t>
   </si>
   <si>
-    <t>Customer</t>
+    <t>Member</t>
   </si>
 </sst>
 </file>
@@ -391,7 +391,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>